<commit_message>
Before the copy data feature.
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="69">
   <si>
     <t>EMSTF Resident Support &amp; Computer Operation Support Services Team Roster</t>
   </si>
@@ -1859,7 +1859,7 @@
         <v>23</v>
       </c>
       <c r="S9" s="25" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="T9" s="25" t="s">
         <v>28</v>
@@ -1911,7 +1911,7 @@
       </c>
       <c r="AJ9" s="26">
         <f>AH9-AG9</f>
-        <v>-11.400000000000006</v>
+        <v>-2.4000000000000057</v>
       </c>
       <c r="AK9" s="26">
         <f>AJ9+AI9</f>
@@ -2220,9 +2220,7 @@
       <c r="P12" s="29"/>
       <c r="Q12" s="29"/>
       <c r="R12" s="29"/>
-      <c r="S12" s="29" t="s">
-        <v>21</v>
-      </c>
+      <c r="S12" s="29"/>
       <c r="T12" s="29"/>
       <c r="U12" s="29"/>
       <c r="V12" s="29"/>

</xml_diff>

<commit_message>
Roster Admin. not working
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -177,14 +177,14 @@
     <t>No. of working day</t>
   </si>
   <si>
-    <t xml:space="preserve">TSANG Ka Shing Gary
+    <t xml:space="preserve">Gary
 ITO1 Extn. 2458</t>
   </si>
   <si>
     <t>O</t>
   </si>
   <si>
-    <t xml:space="preserve">YUNG Kin Shing Tommy
+    <t xml:space="preserve">Tommy
 ITO3 Extn. 2458</t>
   </si>
   <si>
@@ -194,15 +194,15 @@
     <t>d</t>
   </si>
   <si>
-    <t xml:space="preserve">HUEN Kwai-leung Andrew
+    <t xml:space="preserve">Andrew
 ITO4 Extn. 2458</t>
   </si>
   <si>
-    <t xml:space="preserve">LI Chi-wai Joseph
+    <t xml:space="preserve">Joseph
 ITO6 Extn. 2458</t>
   </si>
   <si>
-    <t xml:space="preserve">CHAN Tai-hin Jimmy
+    <t xml:space="preserve">Jimmy
 ITO8 Extn. 2458</t>
   </si>
   <si>

</xml_diff>